<commit_message>
added code for dispatcher
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indra\OneDrive\Documents\UiPath\RoboticEnterpriseFramework\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\indra\OneDrive\Documents\UiPath\IA.0165.InvoiceProcessing_Dispatcher\IA.0165.InvoiceProcessing_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -87,10 +87,6 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -163,6 +159,54 @@
   </si>
   <si>
     <t>9,00,000</t>
+  </si>
+  <si>
+    <t>C:\Users\indra\OneDrive\Desktop\IA.0165.InvoiceProcessing</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Screenshots</t>
+  </si>
+  <si>
+    <t>AI.0165.BasePath</t>
+  </si>
+  <si>
+    <t>BasePath</t>
+  </si>
+  <si>
+    <t>AI.0165.ErrorFolderName</t>
+  </si>
+  <si>
+    <t>AI.0165.InputFolderName</t>
+  </si>
+  <si>
+    <t>AI.0165.ReportFolderName</t>
+  </si>
+  <si>
+    <t>AI.0165.ScreenshotsFolderName</t>
+  </si>
+  <si>
+    <t>ErrorFolderName</t>
+  </si>
+  <si>
+    <t>InputFolderName</t>
+  </si>
+  <si>
+    <t>ReportFolderName</t>
+  </si>
+  <si>
+    <t>ScreenshotsFolderName</t>
+  </si>
+  <si>
+    <t>IA.0165.InvoiceProcessing</t>
   </si>
 </sst>
 </file>
@@ -552,7 +596,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -599,13 +643,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -617,7 +661,7 @@
         <v>21</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1675,18 +1719,18 @@
         <v>5</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="C3" s="3"/>
     </row>
@@ -1711,7 +1755,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
@@ -1733,7 +1777,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1744,7 +1788,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
@@ -1755,13 +1799,13 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B13" s="6">
         <v>2000</v>
@@ -1769,51 +1813,51 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2796,7 +2840,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2815,7 +2859,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2843,11 +2887,61 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3845,5 +3939,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>